<commit_message>
🐳chore(assets): add more subjects
Signed-off-by: Liang Zhang <psychelzh@outlook.com>
</commit_message>
<xml_diff>
--- a/assets/subjects.xlsx
+++ b/assets/subjects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lan94\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lan94\Documents\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB8DAB9-0FC1-48B8-BC99-E2DEC0266709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3608D5EB-05E9-43AD-9B0C-514349EC9F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="1477" windowWidth="15390" windowHeight="9533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>姓名</t>
   </si>
@@ -36,43 +36,82 @@
     <t>年龄</t>
   </si>
   <si>
+    <t>女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>杨舜雅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>李萱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>胡茗恺</t>
+  </si>
+  <si>
+    <t>孙悦媛</t>
+  </si>
+  <si>
+    <t>曾奕然</t>
+  </si>
+  <si>
+    <t>常克帅</t>
+  </si>
+  <si>
+    <t>李逸涵</t>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>董明泽</t>
   </si>
   <si>
     <t>男</t>
   </si>
   <si>
+    <t>黄毅航</t>
+  </si>
+  <si>
+    <t>刘洋</t>
+  </si>
+  <si>
+    <t>女</t>
+  </si>
+  <si>
+    <t>任庆阳</t>
+  </si>
+  <si>
+    <t>耿浩翔</t>
+  </si>
+  <si>
+    <t>张晓瑜</t>
+  </si>
+  <si>
+    <t>申钰嘉</t>
+  </si>
+  <si>
+    <t>郑婉怡</t>
+  </si>
+  <si>
+    <t>薛佳菲</t>
+  </si>
+  <si>
     <t>梁文祺</t>
   </si>
   <si>
-    <t>任庆阳</t>
-  </si>
-  <si>
-    <t>申钰嘉</t>
-  </si>
-  <si>
-    <t>耿浩翔</t>
-  </si>
-  <si>
-    <t>郑婉怡</t>
-  </si>
-  <si>
-    <t>女</t>
-  </si>
-  <si>
-    <t>薛佳菲</t>
-  </si>
-  <si>
     <t>陈昱</t>
   </si>
   <si>
-    <t>刘洋</t>
-  </si>
-  <si>
-    <t>张晓瑜</t>
-  </si>
-  <si>
-    <t>黄毅航</t>
+    <t>刘思潼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛艺惠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -407,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -428,10 +467,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -439,10 +478,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -450,32 +489,32 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -483,43 +522,43 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
         <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
         <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -527,28 +566,128 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>